<commit_message>
Nuevos datasets y cambios TP2
</commit_message>
<xml_diff>
--- a/datasets/grasacerdos.xlsx
+++ b/datasets/grasacerdos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Austral\mcd-reg-adv\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Debora\Dropbox\AustralPosgrado\RegAvanzadaVirtual\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFCFFB2-E70A-40AC-94E9-D4752F41ADC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{56AEE08B-70E7-4B70-949A-1A7739FCE1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A2B32BFB-1C77-457C-8B29-E9EAEB040EAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A2B32BFB-1C77-457C-8B29-E9EAEB040EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Obs</t>
   </si>
@@ -42,17 +43,194 @@
     <t>PV</t>
   </si>
   <si>
+    <t>56,81</t>
+  </si>
+  <si>
+    <t>70,40</t>
+  </si>
+  <si>
+    <t>71,73</t>
+  </si>
+  <si>
+    <t>75,10</t>
+  </si>
+  <si>
+    <t>79,65</t>
+  </si>
+  <si>
+    <t>51,43</t>
+  </si>
+  <si>
+    <t>52,10</t>
+  </si>
+  <si>
+    <t>69,10</t>
+  </si>
+  <si>
+    <t>35,70</t>
+  </si>
+  <si>
+    <t>76,44</t>
+  </si>
+  <si>
     <t>EGD</t>
+  </si>
+  <si>
+    <t>16,19</t>
+  </si>
+  <si>
+    <t>22,00</t>
+  </si>
+  <si>
+    <t>19,52</t>
+  </si>
+  <si>
+    <t>31,00</t>
+  </si>
+  <si>
+    <t>23,58</t>
+  </si>
+  <si>
+    <t>16,58</t>
+  </si>
+  <si>
+    <t>17,20</t>
+  </si>
+  <si>
+    <t>26,70</t>
+  </si>
+  <si>
+    <t>21,60</t>
+  </si>
+  <si>
+    <t>24,51</t>
+  </si>
+  <si>
+    <t>27,51</t>
+  </si>
+  <si>
+    <t>67,90</t>
+  </si>
+  <si>
+    <t>51,61</t>
+  </si>
+  <si>
+    <t>69,40</t>
+  </si>
+  <si>
+    <t>48,93</t>
+  </si>
+  <si>
+    <t>55,02</t>
+  </si>
+  <si>
+    <t>62,70</t>
+  </si>
+  <si>
+    <t>84,00</t>
+  </si>
+  <si>
+    <t>67,50</t>
+  </si>
+  <si>
+    <t>58,62</t>
+  </si>
+  <si>
+    <t>16,21</t>
+  </si>
+  <si>
+    <t>13,80</t>
+  </si>
+  <si>
+    <t>16,43</t>
+  </si>
+  <si>
+    <t>33,60</t>
+  </si>
+  <si>
+    <t>25,07</t>
+  </si>
+  <si>
+    <t>20,52</t>
+  </si>
+  <si>
+    <t>26,20</t>
+  </si>
+  <si>
+    <t>11,50</t>
+  </si>
+  <si>
+    <t>21,50</t>
+  </si>
+  <si>
+    <t>27,26</t>
+  </si>
+  <si>
+    <t>68,58</t>
+  </si>
+  <si>
+    <t>67,10</t>
+  </si>
+  <si>
+    <t>49,10</t>
+  </si>
+  <si>
+    <t>73,80</t>
+  </si>
+  <si>
+    <t>61,40</t>
+  </si>
+  <si>
+    <t>63,44</t>
+  </si>
+  <si>
+    <t>93,00</t>
+  </si>
+  <si>
+    <t>58,90</t>
+  </si>
+  <si>
+    <t>58,70</t>
+  </si>
+  <si>
+    <t>66,45</t>
+  </si>
+  <si>
+    <t>12,60</t>
+  </si>
+  <si>
+    <t>23,30</t>
+  </si>
+  <si>
+    <t>32,46</t>
+  </si>
+  <si>
+    <t>19,90</t>
+  </si>
+  <si>
+    <t>20,48</t>
+  </si>
+  <si>
+    <t>7,29</t>
+  </si>
+  <si>
+    <t>40,90</t>
+  </si>
+  <si>
+    <t>9,21</t>
+  </si>
+  <si>
+    <t>27,60</t>
+  </si>
+  <si>
+    <t>23,27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +240,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,11 +264,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -105,12 +275,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -127,7 +293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -426,15 +592,15 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" style="1"/>
+    <col min="1" max="3" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -442,337 +608,337 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>56.81</v>
-      </c>
-      <c r="C2" s="3">
-        <v>16.190000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>70.400000000000006</v>
-      </c>
-      <c r="C3" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>71.73</v>
-      </c>
-      <c r="C4" s="3">
-        <v>19.52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <v>75.099999999999994</v>
-      </c>
-      <c r="C5" s="3">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
-        <v>79.650000000000006</v>
-      </c>
-      <c r="C6" s="3">
-        <v>23.58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>51.43</v>
-      </c>
-      <c r="C7" s="3">
-        <v>16.579999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
-        <v>52.1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
-        <v>69.099999999999994</v>
-      </c>
-      <c r="C9" s="3">
-        <v>26.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
-        <v>35.700000000000003</v>
-      </c>
-      <c r="C10" s="3">
-        <v>21.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>76.44</v>
-      </c>
-      <c r="C11" s="3">
-        <v>24.51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
-        <v>27.51</v>
-      </c>
-      <c r="C12" s="3">
-        <v>16.21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>67.900000000000006</v>
-      </c>
-      <c r="C13" s="3">
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <v>51.61</v>
-      </c>
-      <c r="C14" s="3">
-        <v>16.43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="C15" s="3">
-        <v>33.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
-        <v>48.93</v>
-      </c>
-      <c r="C16" s="3">
-        <v>25.07</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
-        <v>55.02</v>
-      </c>
-      <c r="C17" s="3">
-        <v>20.52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
-        <v>62.7</v>
-      </c>
-      <c r="C18" s="3">
-        <v>26.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
-        <v>84</v>
-      </c>
-      <c r="C19" s="3">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>67.5</v>
-      </c>
-      <c r="C20" s="3">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>58.62</v>
-      </c>
-      <c r="C21" s="3">
-        <v>27.26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>68.58</v>
-      </c>
-      <c r="C22" s="3">
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="C23" s="3">
-        <v>23.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>49.1</v>
-      </c>
-      <c r="C24" s="3">
-        <v>32.46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
-        <v>73.8</v>
-      </c>
-      <c r="C25" s="3">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
-        <v>61.4</v>
-      </c>
-      <c r="C26" s="3">
-        <v>20.48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
-        <v>63.44</v>
-      </c>
-      <c r="C27" s="3">
-        <v>7.29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
-        <v>93</v>
-      </c>
-      <c r="C28" s="3">
-        <v>40.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>58.9</v>
-      </c>
-      <c r="C29" s="3">
-        <v>9.2100000000000009</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
-        <v>58.7</v>
-      </c>
-      <c r="C30" s="3">
-        <v>27.6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>66.45</v>
-      </c>
-      <c r="C31" s="3">
-        <v>23.27</v>
+      <c r="B31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>